<commit_message>
INA calibration after zap
</commit_message>
<xml_diff>
--- a/IsolatedHardwareTests/teensyPWMtest/pwm_deadtime_and_freq_IPT004.xlsx
+++ b/IsolatedHardwareTests/teensyPWMtest/pwm_deadtime_and_freq_IPT004.xlsx
@@ -2340,8 +2340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>